<commit_message>
update mot so loi ve dang nhap, cap nhap them phan xoa user ,.... cap nhap tin nhan (chua realtime)
</commit_message>
<xml_diff>
--- a/public/excel/33035610.xlsx
+++ b/public/excel/33035610.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
   <si>
     <t>Trường đại học công nghiệp hà nội</t>
   </si>
@@ -87,6 +87,36 @@
   </si>
   <si>
     <t>Kế hoạch</t>
+  </si>
+  <si>
+    <t>2019-11-01</t>
+  </si>
+  <si>
+    <t>2019-11-02</t>
+  </si>
+  <si>
+    <t>2019-11-03</t>
+  </si>
+  <si>
+    <t>2019-11-04</t>
+  </si>
+  <si>
+    <t>2019-11-05</t>
+  </si>
+  <si>
+    <t>2019-11-06</t>
+  </si>
+  <si>
+    <t>2019-11-07</t>
+  </si>
+  <si>
+    <t>2019-11-08</t>
+  </si>
+  <si>
+    <t>2019-11-09</t>
+  </si>
+  <si>
+    <t>2019-11-10</t>
   </si>
 </sst>
 </file>
@@ -114,7 +144,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,6 +154,9 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -132,10 +165,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -437,7 +470,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="R1" sqref="R1"/>
@@ -581,6 +614,186 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>6</v>
+      </c>
+      <c r="I9" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9"/>
+      <c r="M9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <v>6</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10"/>
+      <c r="M10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>6</v>
+      </c>
+      <c r="I11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11"/>
+      <c r="M11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>6</v>
+      </c>
+      <c r="I12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12"/>
+      <c r="M12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="H13">
+        <v>6</v>
+      </c>
+      <c r="I13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13"/>
+      <c r="M13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="H14">
+        <v>6</v>
+      </c>
+      <c r="I14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K14"/>
+      <c r="M14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="H15">
+        <v>6</v>
+      </c>
+      <c r="I15" t="s">
+        <v>30</v>
+      </c>
+      <c r="K15"/>
+      <c r="M15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="H16">
+        <v>6</v>
+      </c>
+      <c r="I16" t="s">
+        <v>31</v>
+      </c>
+      <c r="K16"/>
+      <c r="M16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="B17">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>9</v>
+      </c>
+      <c r="H17">
+        <v>6</v>
+      </c>
+      <c r="I17" t="s">
+        <v>32</v>
+      </c>
+      <c r="K17"/>
+      <c r="M17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
+      </c>
+      <c r="H18">
+        <v>6</v>
+      </c>
+      <c r="I18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K18"/>
+      <c r="M18">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -613,6 +826,46 @@
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="M7:O8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:O18"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>